<commit_message>
schedule xml and xsd
</commit_message>
<xml_diff>
--- a/data/MaraudersInfo.xlsx
+++ b/data/MaraudersInfo.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="1" r:id="rId1"/>
-    <sheet name="Schedule" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="RAW Schedule" sheetId="2" r:id="rId2"/>
+    <sheet name="Parsed Schedule" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="382">
   <si>
     <t>MICHAEL</t>
   </si>
@@ -1126,6 +1126,42 @@
   </si>
   <si>
     <t>position</t>
+  </si>
+  <si>
+    <t>away_score</t>
+  </si>
+  <si>
+    <t>home_score</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>away</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>win</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -1161,17 +1197,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1470,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M91"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1525,7 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
@@ -1505,7 +1550,7 @@
       <c r="D1" t="s">
         <v>369</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>361</v>
       </c>
       <c r="F1" t="s">
@@ -1543,7 +1588,7 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
       <c r="F2">
@@ -1585,7 +1630,7 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>6</v>
       </c>
       <c r="F3">
@@ -1627,7 +1672,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>6</v>
       </c>
       <c r="F4">
@@ -1669,7 +1714,7 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>5</v>
       </c>
       <c r="F5">
@@ -1711,7 +1756,7 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>6</v>
       </c>
       <c r="F6">
@@ -1753,7 +1798,7 @@
       <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7">
@@ -1795,7 +1840,7 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>6</v>
       </c>
       <c r="F8">
@@ -1837,7 +1882,7 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>6</v>
       </c>
       <c r="F9">
@@ -1879,7 +1924,7 @@
       <c r="D10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>6</v>
       </c>
       <c r="F10">
@@ -1921,7 +1966,7 @@
       <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>5</v>
       </c>
       <c r="F11">
@@ -1963,7 +2008,7 @@
       <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>6</v>
       </c>
       <c r="F12">
@@ -2005,7 +2050,7 @@
       <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <v>6</v>
       </c>
       <c r="F13">
@@ -2047,7 +2092,7 @@
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <v>6</v>
       </c>
       <c r="F14">
@@ -2089,7 +2134,7 @@
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>5</v>
       </c>
       <c r="F15">
@@ -2131,7 +2176,7 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <v>6</v>
       </c>
       <c r="F16">
@@ -2173,7 +2218,7 @@
       <c r="D17" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <v>6</v>
       </c>
       <c r="F17">
@@ -2215,7 +2260,7 @@
       <c r="D18" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>5</v>
       </c>
       <c r="F18">
@@ -2257,7 +2302,7 @@
       <c r="D19" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>5</v>
       </c>
       <c r="F19">
@@ -2299,7 +2344,7 @@
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <v>6</v>
       </c>
       <c r="F20">
@@ -2341,7 +2386,7 @@
       <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21">
@@ -2383,7 +2428,7 @@
       <c r="D22" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="2">
         <v>5</v>
       </c>
       <c r="F22">
@@ -2425,7 +2470,7 @@
       <c r="D23" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <v>5</v>
       </c>
       <c r="F23">
@@ -2467,7 +2512,7 @@
       <c r="D24" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <v>6</v>
       </c>
       <c r="F24">
@@ -2509,7 +2554,7 @@
       <c r="D25" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="2">
         <v>5</v>
       </c>
       <c r="F25">
@@ -2551,7 +2596,7 @@
       <c r="D26" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="2">
         <v>5</v>
       </c>
       <c r="F26">
@@ -2593,7 +2638,7 @@
       <c r="D27" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="2">
         <v>6</v>
       </c>
       <c r="F27">
@@ -2635,7 +2680,7 @@
       <c r="D28" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="2">
         <v>6</v>
       </c>
       <c r="F28">
@@ -2677,7 +2722,7 @@
       <c r="D29" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="2">
         <v>5</v>
       </c>
       <c r="F29">
@@ -2719,7 +2764,7 @@
       <c r="D30" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="2">
         <v>5</v>
       </c>
       <c r="F30">
@@ -2761,7 +2806,7 @@
       <c r="D31" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <v>5</v>
       </c>
       <c r="F31">
@@ -2803,7 +2848,7 @@
       <c r="D32" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="2">
         <v>6</v>
       </c>
       <c r="F32">
@@ -2845,7 +2890,7 @@
       <c r="D33" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <v>6</v>
       </c>
       <c r="F33">
@@ -2887,7 +2932,7 @@
       <c r="D34" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="2">
         <v>6</v>
       </c>
       <c r="F34">
@@ -2929,7 +2974,7 @@
       <c r="D35" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="2">
         <v>6</v>
       </c>
       <c r="F35">
@@ -2971,7 +3016,7 @@
       <c r="D36" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="2">
         <v>5</v>
       </c>
       <c r="F36">
@@ -3013,7 +3058,7 @@
       <c r="D37" t="s">
         <v>129</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="2">
         <v>6</v>
       </c>
       <c r="F37">
@@ -3055,7 +3100,7 @@
       <c r="D38" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="2">
         <v>5</v>
       </c>
       <c r="F38">
@@ -3097,7 +3142,7 @@
       <c r="D39" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="2">
         <v>5</v>
       </c>
       <c r="F39">
@@ -3139,7 +3184,7 @@
       <c r="D40" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="2">
         <v>6</v>
       </c>
       <c r="F40">
@@ -3181,7 +3226,7 @@
       <c r="D41" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="2">
         <v>6</v>
       </c>
       <c r="F41">
@@ -3223,7 +3268,7 @@
       <c r="D42" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="2">
         <v>6</v>
       </c>
       <c r="F42">
@@ -3265,7 +3310,7 @@
       <c r="D43" t="s">
         <v>14</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="2">
         <v>6</v>
       </c>
       <c r="F43">
@@ -3307,7 +3352,7 @@
       <c r="D44" t="s">
         <v>166</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="2">
         <v>6</v>
       </c>
       <c r="F44">
@@ -3349,7 +3394,7 @@
       <c r="D45" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="2">
         <v>6</v>
       </c>
       <c r="F45">
@@ -3391,7 +3436,7 @@
       <c r="D46" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="2">
         <v>6</v>
       </c>
       <c r="F46">
@@ -3433,7 +3478,7 @@
       <c r="D47" t="s">
         <v>14</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="2">
         <v>6</v>
       </c>
       <c r="F47">
@@ -3475,7 +3520,7 @@
       <c r="D48" t="s">
         <v>166</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="2">
         <v>6</v>
       </c>
       <c r="F48">
@@ -3517,7 +3562,7 @@
       <c r="D49" t="s">
         <v>166</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="2">
         <v>6</v>
       </c>
       <c r="F49">
@@ -3559,7 +3604,7 @@
       <c r="D50" t="s">
         <v>166</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="2">
         <v>6</v>
       </c>
       <c r="F50">
@@ -3601,7 +3646,7 @@
       <c r="D51" t="s">
         <v>166</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="2">
         <v>6</v>
       </c>
       <c r="F51">
@@ -3643,7 +3688,7 @@
       <c r="D52" t="s">
         <v>166</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="2">
         <v>6</v>
       </c>
       <c r="F52">
@@ -3685,7 +3730,7 @@
       <c r="D53" t="s">
         <v>166</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="2">
         <v>6</v>
       </c>
       <c r="F53">
@@ -3727,7 +3772,7 @@
       <c r="D54" t="s">
         <v>166</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="2">
         <v>6</v>
       </c>
       <c r="F54">
@@ -3769,7 +3814,7 @@
       <c r="D55" t="s">
         <v>166</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="2">
         <v>6</v>
       </c>
       <c r="F55">
@@ -3811,7 +3856,7 @@
       <c r="D56" t="s">
         <v>166</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="2">
         <v>6</v>
       </c>
       <c r="F56">
@@ -3853,7 +3898,7 @@
       <c r="D57" t="s">
         <v>166</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="2">
         <v>6</v>
       </c>
       <c r="F57">
@@ -3895,7 +3940,7 @@
       <c r="D58" t="s">
         <v>14</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="2">
         <v>6</v>
       </c>
       <c r="F58">
@@ -3937,7 +3982,7 @@
       <c r="D59" t="s">
         <v>129</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="2">
         <v>6</v>
       </c>
       <c r="F59">
@@ -3979,7 +4024,7 @@
       <c r="D60" t="s">
         <v>129</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E60" s="2">
         <v>6</v>
       </c>
       <c r="F60">
@@ -4021,7 +4066,7 @@
       <c r="D61" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61" s="2">
         <v>6</v>
       </c>
       <c r="F61">
@@ -4063,7 +4108,7 @@
       <c r="D62" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="2">
         <v>6</v>
       </c>
       <c r="F62">
@@ -4105,7 +4150,7 @@
       <c r="D63" t="s">
         <v>2</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="2">
         <v>5</v>
       </c>
       <c r="F63">
@@ -4147,7 +4192,7 @@
       <c r="D64" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="4">
+      <c r="E64" s="2">
         <v>6</v>
       </c>
       <c r="F64">
@@ -4189,7 +4234,7 @@
       <c r="D65" t="s">
         <v>2</v>
       </c>
-      <c r="E65" s="4">
+      <c r="E65" s="2">
         <v>6</v>
       </c>
       <c r="F65">
@@ -4231,7 +4276,7 @@
       <c r="D66" t="s">
         <v>129</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="2">
         <v>6</v>
       </c>
       <c r="F66">
@@ -4273,7 +4318,7 @@
       <c r="D67" t="s">
         <v>129</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67" s="2">
         <v>6</v>
       </c>
       <c r="F67">
@@ -4315,7 +4360,7 @@
       <c r="D68" t="s">
         <v>129</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="2">
         <v>6</v>
       </c>
       <c r="F68">
@@ -4357,7 +4402,7 @@
       <c r="D69" t="s">
         <v>129</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="2">
         <v>5</v>
       </c>
       <c r="F69">
@@ -4399,7 +4444,7 @@
       <c r="D70" t="s">
         <v>129</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E70" s="2">
         <v>6</v>
       </c>
       <c r="F70">
@@ -4441,7 +4486,7 @@
       <c r="D71" t="s">
         <v>31</v>
       </c>
-      <c r="E71" s="4">
+      <c r="E71" s="2">
         <v>5</v>
       </c>
       <c r="F71">
@@ -4483,7 +4528,7 @@
       <c r="D72" t="s">
         <v>166</v>
       </c>
-      <c r="E72" s="4">
+      <c r="E72" s="2">
         <v>6</v>
       </c>
       <c r="F72">
@@ -4525,7 +4570,7 @@
       <c r="D73" t="s">
         <v>129</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="2">
         <v>6</v>
       </c>
       <c r="F73">
@@ -4567,7 +4612,7 @@
       <c r="D74" t="s">
         <v>166</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="2">
         <v>6</v>
       </c>
       <c r="F74">
@@ -4609,7 +4654,7 @@
       <c r="D75" t="s">
         <v>14</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75" s="2">
         <v>6</v>
       </c>
       <c r="F75">
@@ -4651,7 +4696,7 @@
       <c r="D76" t="s">
         <v>31</v>
       </c>
-      <c r="E76" s="4">
+      <c r="E76" s="2">
         <v>5</v>
       </c>
       <c r="F76">
@@ -4693,7 +4738,7 @@
       <c r="D77" t="s">
         <v>2</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77" s="2">
         <v>6</v>
       </c>
       <c r="F77">
@@ -4735,7 +4780,7 @@
       <c r="D78" t="s">
         <v>44</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78" s="2">
         <v>5</v>
       </c>
       <c r="F78">
@@ -4777,7 +4822,7 @@
       <c r="D79" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="4">
+      <c r="E79" s="2">
         <v>6</v>
       </c>
       <c r="F79">
@@ -4819,7 +4864,7 @@
       <c r="D80" t="s">
         <v>2</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80" s="2">
         <v>5</v>
       </c>
       <c r="F80">
@@ -4861,7 +4906,7 @@
       <c r="D81" t="s">
         <v>44</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E81" s="2">
         <v>5</v>
       </c>
       <c r="F81">
@@ -4903,7 +4948,7 @@
       <c r="D82" t="s">
         <v>129</v>
       </c>
-      <c r="E82" s="4">
+      <c r="E82" s="2">
         <v>6</v>
       </c>
       <c r="F82">
@@ -4945,7 +4990,7 @@
       <c r="D83" t="s">
         <v>2</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="2">
         <v>5</v>
       </c>
       <c r="F83">
@@ -4987,7 +5032,7 @@
       <c r="D84" t="s">
         <v>129</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="2">
         <v>6</v>
       </c>
       <c r="F84">
@@ -5029,7 +5074,7 @@
       <c r="D85" t="s">
         <v>20</v>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="2">
         <v>5</v>
       </c>
       <c r="F85">
@@ -5071,7 +5116,7 @@
       <c r="D86" t="s">
         <v>129</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86" s="2">
         <v>6</v>
       </c>
       <c r="F86">
@@ -5113,7 +5158,7 @@
       <c r="D87" t="s">
         <v>166</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87" s="2">
         <v>5</v>
       </c>
       <c r="F87">
@@ -5155,7 +5200,7 @@
       <c r="D88" t="s">
         <v>2</v>
       </c>
-      <c r="E88" s="4">
+      <c r="E88" s="2">
         <v>6</v>
       </c>
       <c r="F88">
@@ -5197,7 +5242,7 @@
       <c r="D89" t="s">
         <v>166</v>
       </c>
-      <c r="E89" s="4">
+      <c r="E89" s="2">
         <v>6</v>
       </c>
       <c r="F89">
@@ -5239,7 +5284,7 @@
       <c r="D90" t="s">
         <v>2</v>
       </c>
-      <c r="E90" s="4">
+      <c r="E90" s="2">
         <v>5</v>
       </c>
       <c r="F90">
@@ -5281,7 +5326,7 @@
       <c r="D91" t="s">
         <v>44</v>
       </c>
-      <c r="E91" s="4">
+      <c r="E91" s="2">
         <v>5</v>
       </c>
       <c r="F91">
@@ -5320,8 +5365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7380,262 +7425,267 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:E91"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="4.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="1"/>
-    </row>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="2"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="1"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="1"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="1"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E53" s="1"/>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E75" s="1"/>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E79" s="2"/>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="1"/>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" s="1"/>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="1"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G2" t="s">
+        <v>377</v>
+      </c>
+      <c r="I2" t="str">
+        <f>"&lt;game "&amp;$A$1&amp;"="""&amp;TRIM(A2)&amp;"""&gt; &lt;"&amp;$B$1&amp;" team="""&amp;TRIM(B2)&amp;""" score="""&amp;C2&amp;"""&gt;&lt;/"&amp;$B$1&amp;"&gt; &lt;"&amp;$D$1&amp;" team="""&amp;TRIM(D2)&amp;""" score="""&amp;E2&amp;"""&gt;&lt;/"&amp;$D$1&amp;"&gt; &lt;"&amp;$F$1&amp;"&gt;"&amp;F2&amp;"&lt;/"&amp;$F$1&amp;"&gt; &lt;"&amp;$G$1&amp;"&gt;"&amp;G2&amp;"&lt;/"&amp;$G$1&amp;"&gt; &lt;/game&gt;"</f>
+        <v>&lt;game date="Sep. 5"&gt; &lt;away team="McMaster" score="26"&gt;&lt;/away&gt; &lt;home team="Queen's" score="2"&gt;&lt;/home&gt; &lt;status&gt;final&lt;/status&gt; &lt;result&gt;win&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>380</v>
+      </c>
+      <c r="G3" t="s">
+        <v>379</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I9" si="0">"&lt;game "&amp;$A$1&amp;"="""&amp;TRIM(A3)&amp;"""&gt; &lt;"&amp;$B$1&amp;" team="""&amp;TRIM(B3)&amp;""" score="""&amp;C3&amp;"""&gt;&lt;/"&amp;$B$1&amp;"&gt; &lt;"&amp;$D$1&amp;" team="""&amp;TRIM(D3)&amp;""" score="""&amp;E3&amp;"""&gt;&lt;/"&amp;$D$1&amp;"&gt; &lt;"&amp;$F$1&amp;"&gt;"&amp;F3&amp;"&lt;/"&amp;$F$1&amp;"&gt; &lt;"&amp;$G$1&amp;"&gt;"&amp;G3&amp;"&lt;/"&amp;$G$1&amp;"&gt; &lt;/game&gt;"</f>
+        <v>&lt;game date="Sep. 10"&gt; &lt;away team="Western" score="48"&gt;&lt;/away&gt; &lt;home team="McMaster" score="21"&gt;&lt;/home&gt; &lt;status&gt;final&lt;/status&gt; &lt;result&gt;loss&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" t="s">
+        <v>320</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>380</v>
+      </c>
+      <c r="G4" t="s">
+        <v>377</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;game date="Sep. 17"&gt; &lt;away team="McMaster" score="21"&gt;&lt;/away&gt; &lt;home team="Windsor" score="19"&gt;&lt;/home&gt; &lt;status&gt;final&lt;/status&gt; &lt;result&gt;win&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C5">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E5">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" t="s">
+        <v>377</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;game date="Sep. 24"&gt; &lt;away team="McMaster" score="37"&gt;&lt;/away&gt; &lt;home team="Guelph" score="13"&gt;&lt;/home&gt; &lt;status&gt;final&lt;/status&gt; &lt;result&gt;win&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E6">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>380</v>
+      </c>
+      <c r="G6" t="s">
+        <v>377</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;game date="Oct. 1"&gt; &lt;away team="Waterloo" score="20"&gt;&lt;/away&gt; &lt;home team="McMaster" score="46"&gt;&lt;/home&gt; &lt;status&gt;final&lt;/status&gt; &lt;result&gt;win&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>320</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>380</v>
+      </c>
+      <c r="G7" t="s">
+        <v>377</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;game date="Oct. 6"&gt; &lt;away team="Toronto" score="14"&gt;&lt;/away&gt; &lt;home team="McMaster" score="50"&gt;&lt;/home&gt; &lt;status&gt;final&lt;/status&gt; &lt;result&gt;win&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>380</v>
+      </c>
+      <c r="G8" t="s">
+        <v>377</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;game date="Oct. 15"&gt; &lt;away team="McMaster" score="25"&gt;&lt;/away&gt; &lt;home team="Laurier" score="6"&gt;&lt;/home&gt; &lt;status&gt;final&lt;/status&gt; &lt;result&gt;win&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>349</v>
+      </c>
+      <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E9" t="s">
+        <v>378</v>
+      </c>
+      <c r="F9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G9" t="s">
+        <v>378</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;game date="Oct. 22"&gt; &lt;away team="Ottawa" score="na"&gt;&lt;/away&gt; &lt;home team="McMaster" score="na"&gt;&lt;/home&gt; &lt;status&gt;Pending&lt;/status&gt; &lt;result&gt;na&lt;/result&gt; &lt;/game&gt;</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:D1048576 E1 G1:G9 E9:F9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"McMaster "</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>